<commit_message>
add annuaire package 9a54fadd8c384bd860109498b2e0ce94264a6c4f
</commit_message>
<xml_diff>
--- a/ig/nr-update-annuaire/StructureDefinition-gap-bundle-reponse-demande-consult-dispo.xlsx
+++ b/ig/nr-update-annuaire/StructureDefinition-gap-bundle-reponse-demande-consult-dispo.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13267" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13267" uniqueCount="651">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-07T15:59:24+00:00</t>
+    <t>2024-04-11T12:15:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,7 +69,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>ANS (https://esante.gouv.fr)</t>
   </si>
   <si>
     <t>Jurisdiction</t>
@@ -902,7 +902,7 @@
     <t>Bundle.entry:Slot.resource</t>
   </si>
   <si>
-    <t xml:space="preserve">Slot {http://interopsante.org/fhir/StructureDefinition/FrSlot}
+    <t xml:space="preserve">Slot {https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-slot}
 </t>
   </si>
   <si>
@@ -910,10 +910,6 @@
   </si>
   <si>
     <t>A slot of time on a schedule that may be available for booking appointments.</t>
-  </si>
-  <si>
-    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
   </si>
   <si>
     <t>Bundle.entry:Slot.search</t>
@@ -1022,7 +1018,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Schedule {http://interopsante.org/fhir/StructureDefinition/FrSchedule}
+    <t xml:space="preserve">Schedule {https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-schedule}
 </t>
   </si>
   <si>
@@ -1138,7 +1134,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Patient {http://interopsante.org/fhir/StructureDefinition/FrPatient}
+    <t xml:space="preserve">Patient {https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-patient}
 </t>
   </si>
   <si>
@@ -1580,7 +1576,7 @@
     <t>Bundle.entry:Location.resource</t>
   </si>
   <si>
-    <t xml:space="preserve">Location {http://interopsante.org/fhir/StructureDefinition/FrLocation}
+    <t xml:space="preserve">Location {https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-location}
 </t>
   </si>
   <si>
@@ -1692,7 +1688,7 @@
     <t>Bundle.entry:HealthcareService.resource</t>
   </si>
   <si>
-    <t xml:space="preserve">HealthcareService {http://interopsante.org/fhir/StructureDefinition/FrHealthcareService}
+    <t xml:space="preserve">HealthcareService {https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-healthcare-service}
 </t>
   </si>
   <si>
@@ -1814,10 +1810,6 @@
     <t>A formally or informally recognized grouping of people or organizations formed for the purpose of achieving some form of collective action.  Includes companies, institutions, corporations, departments, community groups, healthcare practice groups, payer/insurer, etc.</t>
   </si>
   <si>
-    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}org-1:The organization SHALL at least have a name or an identifier, and possibly more than one {(identifier.count() + name.count()) &gt; 0}</t>
-  </si>
-  <si>
     <t>(also see master files messages)</t>
   </si>
   <si>
@@ -1923,7 +1915,7 @@
     <t>Bundle.entry:RelatedPerson.resource</t>
   </si>
   <si>
-    <t xml:space="preserve">RelatedPerson {http://interopsante.org/fhir/StructureDefinition/FrRelatedPerson}
+    <t xml:space="preserve">RelatedPerson {https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-related-person}
 </t>
   </si>
   <si>
@@ -8623,7 +8615,7 @@
         <v>77</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>285</v>
+        <v>77</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>77</v>
@@ -8640,7 +8632,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B56" t="s" s="2">
         <v>203</v>
@@ -8752,7 +8744,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B57" t="s" s="2">
         <v>207</v>
@@ -8864,7 +8856,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B58" t="s" s="2">
         <v>208</v>
@@ -8978,7 +8970,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B59" t="s" s="2">
         <v>209</v>
@@ -9094,7 +9086,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B60" t="s" s="2">
         <v>210</v>
@@ -9140,7 +9132,7 @@
         <v>77</v>
       </c>
       <c r="S60" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T60" t="s" s="2">
         <v>77</v>
@@ -9208,7 +9200,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B61" t="s" s="2">
         <v>216</v>
@@ -9322,7 +9314,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B62" t="s" s="2">
         <v>221</v>
@@ -9434,7 +9426,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B63" t="s" s="2">
         <v>225</v>
@@ -9546,7 +9538,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B64" t="s" s="2">
         <v>226</v>
@@ -9660,7 +9652,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B65" t="s" s="2">
         <v>227</v>
@@ -9776,7 +9768,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B66" t="s" s="2">
         <v>228</v>
@@ -9890,7 +9882,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B67" t="s" s="2">
         <v>233</v>
@@ -10004,7 +9996,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B68" t="s" s="2">
         <v>237</v>
@@ -10118,7 +10110,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B69" t="s" s="2">
         <v>240</v>
@@ -10232,7 +10224,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B70" t="s" s="2">
         <v>243</v>
@@ -10346,7 +10338,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B71" t="s" s="2">
         <v>246</v>
@@ -10460,7 +10452,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B72" t="s" s="2">
         <v>249</v>
@@ -10572,7 +10564,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B73" t="s" s="2">
         <v>253</v>
@@ -10684,7 +10676,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B74" t="s" s="2">
         <v>254</v>
@@ -10798,7 +10790,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B75" t="s" s="2">
         <v>255</v>
@@ -10914,7 +10906,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B76" t="s" s="2">
         <v>256</v>
@@ -11028,7 +11020,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B77" t="s" s="2">
         <v>259</v>
@@ -11142,7 +11134,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B78" t="s" s="2">
         <v>262</v>
@@ -11256,7 +11248,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B79" t="s" s="2">
         <v>266</v>
@@ -11370,7 +11362,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B80" t="s" s="2">
         <v>270</v>
@@ -11484,13 +11476,13 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B81" t="s" s="2">
         <v>183</v>
       </c>
       <c r="C81" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D81" t="s" s="2">
         <v>77</v>
@@ -11598,7 +11590,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B82" t="s" s="2">
         <v>188</v>
@@ -11710,7 +11702,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B83" t="s" s="2">
         <v>189</v>
@@ -11824,7 +11816,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B84" t="s" s="2">
         <v>190</v>
@@ -11940,7 +11932,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B85" t="s" s="2">
         <v>191</v>
@@ -12052,7 +12044,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B86" t="s" s="2">
         <v>194</v>
@@ -12166,14 +12158,14 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B87" t="s" s="2">
         <v>198</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" t="s" s="2">
@@ -12192,13 +12184,13 @@
         <v>77</v>
       </c>
       <c r="K87" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="L87" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="L87" t="s" s="2">
+      <c r="M87" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="M87" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="N87" s="2"/>
       <c r="O87" s="2"/>
@@ -12261,7 +12253,7 @@
         <v>77</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>285</v>
+        <v>77</v>
       </c>
       <c r="AK87" t="s" s="2">
         <v>77</v>
@@ -12278,7 +12270,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B88" t="s" s="2">
         <v>203</v>
@@ -12390,7 +12382,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B89" t="s" s="2">
         <v>207</v>
@@ -12502,7 +12494,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B90" t="s" s="2">
         <v>208</v>
@@ -12616,7 +12608,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B91" t="s" s="2">
         <v>209</v>
@@ -12732,7 +12724,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B92" t="s" s="2">
         <v>210</v>
@@ -12778,7 +12770,7 @@
         <v>77</v>
       </c>
       <c r="S92" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T92" t="s" s="2">
         <v>77</v>
@@ -12846,7 +12838,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B93" t="s" s="2">
         <v>216</v>
@@ -12960,7 +12952,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B94" t="s" s="2">
         <v>221</v>
@@ -13072,7 +13064,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B95" t="s" s="2">
         <v>225</v>
@@ -13184,7 +13176,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B96" t="s" s="2">
         <v>226</v>
@@ -13298,7 +13290,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B97" t="s" s="2">
         <v>227</v>
@@ -13414,7 +13406,7 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B98" t="s" s="2">
         <v>228</v>
@@ -13528,7 +13520,7 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B99" t="s" s="2">
         <v>233</v>
@@ -13642,7 +13634,7 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B100" t="s" s="2">
         <v>237</v>
@@ -13756,7 +13748,7 @@
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B101" t="s" s="2">
         <v>240</v>
@@ -13870,7 +13862,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B102" t="s" s="2">
         <v>243</v>
@@ -13984,7 +13976,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B103" t="s" s="2">
         <v>246</v>
@@ -14098,7 +14090,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B104" t="s" s="2">
         <v>249</v>
@@ -14210,7 +14202,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B105" t="s" s="2">
         <v>253</v>
@@ -14322,7 +14314,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B106" t="s" s="2">
         <v>254</v>
@@ -14436,7 +14428,7 @@
     </row>
     <row r="107">
       <c r="A107" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B107" t="s" s="2">
         <v>255</v>
@@ -14552,7 +14544,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B108" t="s" s="2">
         <v>256</v>
@@ -14666,7 +14658,7 @@
     </row>
     <row r="109">
       <c r="A109" t="s" s="2">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B109" t="s" s="2">
         <v>259</v>
@@ -14780,7 +14772,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B110" t="s" s="2">
         <v>262</v>
@@ -14894,7 +14886,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s" s="2">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B111" t="s" s="2">
         <v>266</v>
@@ -15008,7 +15000,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B112" t="s" s="2">
         <v>270</v>
@@ -15122,13 +15114,13 @@
     </row>
     <row r="113">
       <c r="A113" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B113" t="s" s="2">
         <v>183</v>
       </c>
       <c r="C113" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D113" t="s" s="2">
         <v>77</v>
@@ -15236,7 +15228,7 @@
     </row>
     <row r="114">
       <c r="A114" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B114" t="s" s="2">
         <v>188</v>
@@ -15348,7 +15340,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B115" t="s" s="2">
         <v>189</v>
@@ -15462,7 +15454,7 @@
     </row>
     <row r="116">
       <c r="A116" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B116" t="s" s="2">
         <v>190</v>
@@ -15578,7 +15570,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B117" t="s" s="2">
         <v>191</v>
@@ -15690,7 +15682,7 @@
     </row>
     <row r="118">
       <c r="A118" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B118" t="s" s="2">
         <v>194</v>
@@ -15804,14 +15796,14 @@
     </row>
     <row r="119">
       <c r="A119" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B119" t="s" s="2">
         <v>198</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" t="s" s="2">
@@ -15830,13 +15822,13 @@
         <v>77</v>
       </c>
       <c r="K119" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="L119" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="L119" t="s" s="2">
+      <c r="M119" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="M119" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="N119" s="2"/>
       <c r="O119" s="2"/>
@@ -15899,16 +15891,16 @@
         <v>77</v>
       </c>
       <c r="AJ119" t="s" s="2">
-        <v>285</v>
+        <v>77</v>
       </c>
       <c r="AK119" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AL119" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="AM119" t="s" s="2">
         <v>362</v>
-      </c>
-      <c r="AM119" t="s" s="2">
-        <v>363</v>
       </c>
       <c r="AN119" t="s" s="2">
         <v>77</v>
@@ -15916,7 +15908,7 @@
     </row>
     <row r="120">
       <c r="A120" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B120" t="s" s="2">
         <v>203</v>
@@ -16028,7 +16020,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B121" t="s" s="2">
         <v>207</v>
@@ -16140,7 +16132,7 @@
     </row>
     <row r="122">
       <c r="A122" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B122" t="s" s="2">
         <v>208</v>
@@ -16254,7 +16246,7 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B123" t="s" s="2">
         <v>209</v>
@@ -16370,7 +16362,7 @@
     </row>
     <row r="124">
       <c r="A124" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B124" t="s" s="2">
         <v>210</v>
@@ -16416,7 +16408,7 @@
         <v>77</v>
       </c>
       <c r="S124" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T124" t="s" s="2">
         <v>77</v>
@@ -16484,7 +16476,7 @@
     </row>
     <row r="125">
       <c r="A125" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B125" t="s" s="2">
         <v>216</v>
@@ -16598,7 +16590,7 @@
     </row>
     <row r="126">
       <c r="A126" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B126" t="s" s="2">
         <v>221</v>
@@ -16710,7 +16702,7 @@
     </row>
     <row r="127">
       <c r="A127" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B127" t="s" s="2">
         <v>225</v>
@@ -16822,7 +16814,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B128" t="s" s="2">
         <v>226</v>
@@ -16936,7 +16928,7 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B129" t="s" s="2">
         <v>227</v>
@@ -17052,7 +17044,7 @@
     </row>
     <row r="130">
       <c r="A130" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B130" t="s" s="2">
         <v>228</v>
@@ -17166,7 +17158,7 @@
     </row>
     <row r="131">
       <c r="A131" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B131" t="s" s="2">
         <v>233</v>
@@ -17280,7 +17272,7 @@
     </row>
     <row r="132">
       <c r="A132" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B132" t="s" s="2">
         <v>237</v>
@@ -17394,7 +17386,7 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="2">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B133" t="s" s="2">
         <v>240</v>
@@ -17508,7 +17500,7 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B134" t="s" s="2">
         <v>243</v>
@@ -17622,7 +17614,7 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="2">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B135" t="s" s="2">
         <v>246</v>
@@ -17736,7 +17728,7 @@
     </row>
     <row r="136">
       <c r="A136" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B136" t="s" s="2">
         <v>249</v>
@@ -17848,7 +17840,7 @@
     </row>
     <row r="137">
       <c r="A137" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B137" t="s" s="2">
         <v>253</v>
@@ -17960,7 +17952,7 @@
     </row>
     <row r="138">
       <c r="A138" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B138" t="s" s="2">
         <v>254</v>
@@ -18074,7 +18066,7 @@
     </row>
     <row r="139">
       <c r="A139" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B139" t="s" s="2">
         <v>255</v>
@@ -18190,7 +18182,7 @@
     </row>
     <row r="140">
       <c r="A140" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B140" t="s" s="2">
         <v>256</v>
@@ -18304,7 +18296,7 @@
     </row>
     <row r="141">
       <c r="A141" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B141" t="s" s="2">
         <v>259</v>
@@ -18418,7 +18410,7 @@
     </row>
     <row r="142">
       <c r="A142" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B142" t="s" s="2">
         <v>262</v>
@@ -18532,7 +18524,7 @@
     </row>
     <row r="143">
       <c r="A143" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B143" t="s" s="2">
         <v>266</v>
@@ -18646,7 +18638,7 @@
     </row>
     <row r="144">
       <c r="A144" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B144" t="s" s="2">
         <v>270</v>
@@ -18760,13 +18752,13 @@
     </row>
     <row r="145">
       <c r="A145" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B145" t="s" s="2">
         <v>183</v>
       </c>
       <c r="C145" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D145" t="s" s="2">
         <v>77</v>
@@ -18874,7 +18866,7 @@
     </row>
     <row r="146">
       <c r="A146" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B146" t="s" s="2">
         <v>188</v>
@@ -18986,7 +18978,7 @@
     </row>
     <row r="147">
       <c r="A147" t="s" s="2">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B147" t="s" s="2">
         <v>189</v>
@@ -19100,7 +19092,7 @@
     </row>
     <row r="148">
       <c r="A148" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B148" t="s" s="2">
         <v>190</v>
@@ -19216,7 +19208,7 @@
     </row>
     <row r="149">
       <c r="A149" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B149" t="s" s="2">
         <v>191</v>
@@ -19328,7 +19320,7 @@
     </row>
     <row r="150">
       <c r="A150" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B150" t="s" s="2">
         <v>194</v>
@@ -19442,7 +19434,7 @@
     </row>
     <row r="151">
       <c r="A151" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B151" t="s" s="2">
         <v>198</v>
@@ -19468,13 +19460,13 @@
         <v>77</v>
       </c>
       <c r="K151" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="L151" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="L151" t="s" s="2">
+      <c r="M151" t="s" s="2">
         <v>398</v>
-      </c>
-      <c r="M151" t="s" s="2">
-        <v>399</v>
       </c>
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
@@ -19537,13 +19529,13 @@
         <v>77</v>
       </c>
       <c r="AJ151" t="s" s="2">
-        <v>285</v>
+        <v>77</v>
       </c>
       <c r="AK151" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="AL151" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="AL151" t="s" s="2">
-        <v>401</v>
       </c>
       <c r="AM151" t="s" s="2">
         <v>77</v>
@@ -19554,7 +19546,7 @@
     </row>
     <row r="152">
       <c r="A152" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B152" t="s" s="2">
         <v>203</v>
@@ -19666,7 +19658,7 @@
     </row>
     <row r="153">
       <c r="A153" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B153" t="s" s="2">
         <v>207</v>
@@ -19778,7 +19770,7 @@
     </row>
     <row r="154">
       <c r="A154" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B154" t="s" s="2">
         <v>208</v>
@@ -19892,7 +19884,7 @@
     </row>
     <row r="155">
       <c r="A155" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B155" t="s" s="2">
         <v>209</v>
@@ -20008,7 +20000,7 @@
     </row>
     <row r="156">
       <c r="A156" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B156" t="s" s="2">
         <v>210</v>
@@ -20054,7 +20046,7 @@
         <v>77</v>
       </c>
       <c r="S156" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T156" t="s" s="2">
         <v>77</v>
@@ -20122,7 +20114,7 @@
     </row>
     <row r="157">
       <c r="A157" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B157" t="s" s="2">
         <v>216</v>
@@ -20236,7 +20228,7 @@
     </row>
     <row r="158">
       <c r="A158" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B158" t="s" s="2">
         <v>221</v>
@@ -20348,7 +20340,7 @@
     </row>
     <row r="159">
       <c r="A159" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B159" t="s" s="2">
         <v>225</v>
@@ -20460,7 +20452,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B160" t="s" s="2">
         <v>226</v>
@@ -20574,7 +20566,7 @@
     </row>
     <row r="161">
       <c r="A161" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B161" t="s" s="2">
         <v>227</v>
@@ -20690,7 +20682,7 @@
     </row>
     <row r="162">
       <c r="A162" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B162" t="s" s="2">
         <v>228</v>
@@ -20804,7 +20796,7 @@
     </row>
     <row r="163">
       <c r="A163" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B163" t="s" s="2">
         <v>233</v>
@@ -20918,7 +20910,7 @@
     </row>
     <row r="164">
       <c r="A164" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B164" t="s" s="2">
         <v>237</v>
@@ -21032,7 +21024,7 @@
     </row>
     <row r="165">
       <c r="A165" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B165" t="s" s="2">
         <v>240</v>
@@ -21146,7 +21138,7 @@
     </row>
     <row r="166">
       <c r="A166" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B166" t="s" s="2">
         <v>243</v>
@@ -21260,7 +21252,7 @@
     </row>
     <row r="167">
       <c r="A167" t="s" s="2">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B167" t="s" s="2">
         <v>246</v>
@@ -21374,7 +21366,7 @@
     </row>
     <row r="168">
       <c r="A168" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B168" t="s" s="2">
         <v>249</v>
@@ -21486,7 +21478,7 @@
     </row>
     <row r="169">
       <c r="A169" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B169" t="s" s="2">
         <v>253</v>
@@ -21598,7 +21590,7 @@
     </row>
     <row r="170">
       <c r="A170" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B170" t="s" s="2">
         <v>254</v>
@@ -21712,7 +21704,7 @@
     </row>
     <row r="171">
       <c r="A171" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B171" t="s" s="2">
         <v>255</v>
@@ -21828,7 +21820,7 @@
     </row>
     <row r="172">
       <c r="A172" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B172" t="s" s="2">
         <v>256</v>
@@ -21942,7 +21934,7 @@
     </row>
     <row r="173">
       <c r="A173" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B173" t="s" s="2">
         <v>259</v>
@@ -22056,7 +22048,7 @@
     </row>
     <row r="174">
       <c r="A174" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B174" t="s" s="2">
         <v>262</v>
@@ -22170,7 +22162,7 @@
     </row>
     <row r="175">
       <c r="A175" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B175" t="s" s="2">
         <v>266</v>
@@ -22284,7 +22276,7 @@
     </row>
     <row r="176">
       <c r="A176" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B176" t="s" s="2">
         <v>270</v>
@@ -22398,13 +22390,13 @@
     </row>
     <row r="177">
       <c r="A177" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B177" t="s" s="2">
         <v>183</v>
       </c>
       <c r="C177" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D177" t="s" s="2">
         <v>77</v>
@@ -22512,7 +22504,7 @@
     </row>
     <row r="178">
       <c r="A178" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B178" t="s" s="2">
         <v>188</v>
@@ -22624,7 +22616,7 @@
     </row>
     <row r="179">
       <c r="A179" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B179" t="s" s="2">
         <v>189</v>
@@ -22738,7 +22730,7 @@
     </row>
     <row r="180">
       <c r="A180" t="s" s="2">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B180" t="s" s="2">
         <v>190</v>
@@ -22854,7 +22846,7 @@
     </row>
     <row r="181">
       <c r="A181" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B181" t="s" s="2">
         <v>191</v>
@@ -22966,7 +22958,7 @@
     </row>
     <row r="182">
       <c r="A182" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B182" t="s" s="2">
         <v>194</v>
@@ -23080,7 +23072,7 @@
     </row>
     <row r="183">
       <c r="A183" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B183" t="s" s="2">
         <v>198</v>
@@ -23106,13 +23098,13 @@
         <v>77</v>
       </c>
       <c r="K183" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="L183" t="s" s="2">
         <v>435</v>
       </c>
-      <c r="L183" t="s" s="2">
+      <c r="M183" t="s" s="2">
         <v>436</v>
-      </c>
-      <c r="M183" t="s" s="2">
-        <v>437</v>
       </c>
       <c r="N183" s="2"/>
       <c r="O183" s="2"/>
@@ -23175,13 +23167,13 @@
         <v>77</v>
       </c>
       <c r="AJ183" t="s" s="2">
-        <v>285</v>
+        <v>77</v>
       </c>
       <c r="AK183" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="AL183" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="AL183" t="s" s="2">
-        <v>401</v>
       </c>
       <c r="AM183" t="s" s="2">
         <v>77</v>
@@ -23192,7 +23184,7 @@
     </row>
     <row r="184">
       <c r="A184" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B184" t="s" s="2">
         <v>203</v>
@@ -23304,7 +23296,7 @@
     </row>
     <row r="185">
       <c r="A185" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B185" t="s" s="2">
         <v>207</v>
@@ -23416,7 +23408,7 @@
     </row>
     <row r="186">
       <c r="A186" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B186" t="s" s="2">
         <v>208</v>
@@ -23530,7 +23522,7 @@
     </row>
     <row r="187">
       <c r="A187" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B187" t="s" s="2">
         <v>209</v>
@@ -23646,7 +23638,7 @@
     </row>
     <row r="188">
       <c r="A188" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B188" t="s" s="2">
         <v>210</v>
@@ -23692,7 +23684,7 @@
         <v>77</v>
       </c>
       <c r="S188" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T188" t="s" s="2">
         <v>77</v>
@@ -23760,7 +23752,7 @@
     </row>
     <row r="189">
       <c r="A189" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B189" t="s" s="2">
         <v>216</v>
@@ -23874,7 +23866,7 @@
     </row>
     <row r="190">
       <c r="A190" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B190" t="s" s="2">
         <v>221</v>
@@ -23986,7 +23978,7 @@
     </row>
     <row r="191">
       <c r="A191" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B191" t="s" s="2">
         <v>225</v>
@@ -24098,7 +24090,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B192" t="s" s="2">
         <v>226</v>
@@ -24212,7 +24204,7 @@
     </row>
     <row r="193">
       <c r="A193" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B193" t="s" s="2">
         <v>227</v>
@@ -24328,7 +24320,7 @@
     </row>
     <row r="194">
       <c r="A194" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B194" t="s" s="2">
         <v>228</v>
@@ -24442,7 +24434,7 @@
     </row>
     <row r="195">
       <c r="A195" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B195" t="s" s="2">
         <v>233</v>
@@ -24556,7 +24548,7 @@
     </row>
     <row r="196">
       <c r="A196" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B196" t="s" s="2">
         <v>237</v>
@@ -24670,7 +24662,7 @@
     </row>
     <row r="197">
       <c r="A197" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B197" t="s" s="2">
         <v>240</v>
@@ -24784,7 +24776,7 @@
     </row>
     <row r="198">
       <c r="A198" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B198" t="s" s="2">
         <v>243</v>
@@ -24898,7 +24890,7 @@
     </row>
     <row r="199">
       <c r="A199" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B199" t="s" s="2">
         <v>246</v>
@@ -25012,7 +25004,7 @@
     </row>
     <row r="200">
       <c r="A200" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B200" t="s" s="2">
         <v>249</v>
@@ -25124,7 +25116,7 @@
     </row>
     <row r="201">
       <c r="A201" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B201" t="s" s="2">
         <v>253</v>
@@ -25236,7 +25228,7 @@
     </row>
     <row r="202">
       <c r="A202" t="s" s="2">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B202" t="s" s="2">
         <v>254</v>
@@ -25350,7 +25342,7 @@
     </row>
     <row r="203">
       <c r="A203" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B203" t="s" s="2">
         <v>255</v>
@@ -25466,7 +25458,7 @@
     </row>
     <row r="204">
       <c r="A204" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B204" t="s" s="2">
         <v>256</v>
@@ -25580,7 +25572,7 @@
     </row>
     <row r="205">
       <c r="A205" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B205" t="s" s="2">
         <v>259</v>
@@ -25694,7 +25686,7 @@
     </row>
     <row r="206">
       <c r="A206" t="s" s="2">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B206" t="s" s="2">
         <v>262</v>
@@ -25808,7 +25800,7 @@
     </row>
     <row r="207">
       <c r="A207" t="s" s="2">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B207" t="s" s="2">
         <v>266</v>
@@ -25922,7 +25914,7 @@
     </row>
     <row r="208">
       <c r="A208" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B208" t="s" s="2">
         <v>270</v>
@@ -26036,13 +26028,13 @@
     </row>
     <row r="209">
       <c r="A209" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B209" t="s" s="2">
         <v>183</v>
       </c>
       <c r="C209" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D209" t="s" s="2">
         <v>77</v>
@@ -26150,7 +26142,7 @@
     </row>
     <row r="210">
       <c r="A210" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B210" t="s" s="2">
         <v>188</v>
@@ -26262,7 +26254,7 @@
     </row>
     <row r="211">
       <c r="A211" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B211" t="s" s="2">
         <v>189</v>
@@ -26376,7 +26368,7 @@
     </row>
     <row r="212">
       <c r="A212" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B212" t="s" s="2">
         <v>190</v>
@@ -26492,7 +26484,7 @@
     </row>
     <row r="213">
       <c r="A213" t="s" s="2">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B213" t="s" s="2">
         <v>191</v>
@@ -26604,7 +26596,7 @@
     </row>
     <row r="214">
       <c r="A214" t="s" s="2">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B214" t="s" s="2">
         <v>194</v>
@@ -26718,7 +26710,7 @@
     </row>
     <row r="215">
       <c r="A215" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B215" t="s" s="2">
         <v>198</v>
@@ -26744,7 +26736,7 @@
         <v>88</v>
       </c>
       <c r="K215" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L215" t="s" s="2">
         <v>200</v>
@@ -26830,7 +26822,7 @@
     </row>
     <row r="216">
       <c r="A216" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B216" t="s" s="2">
         <v>203</v>
@@ -26942,7 +26934,7 @@
     </row>
     <row r="217">
       <c r="A217" t="s" s="2">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B217" t="s" s="2">
         <v>207</v>
@@ -27054,7 +27046,7 @@
     </row>
     <row r="218">
       <c r="A218" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B218" t="s" s="2">
         <v>208</v>
@@ -27168,7 +27160,7 @@
     </row>
     <row r="219">
       <c r="A219" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B219" t="s" s="2">
         <v>209</v>
@@ -27284,7 +27276,7 @@
     </row>
     <row r="220">
       <c r="A220" t="s" s="2">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B220" t="s" s="2">
         <v>210</v>
@@ -27330,7 +27322,7 @@
         <v>77</v>
       </c>
       <c r="S220" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T220" t="s" s="2">
         <v>77</v>
@@ -27398,7 +27390,7 @@
     </row>
     <row r="221">
       <c r="A221" t="s" s="2">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B221" t="s" s="2">
         <v>216</v>
@@ -27512,7 +27504,7 @@
     </row>
     <row r="222">
       <c r="A222" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B222" t="s" s="2">
         <v>221</v>
@@ -27624,7 +27616,7 @@
     </row>
     <row r="223">
       <c r="A223" t="s" s="2">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B223" t="s" s="2">
         <v>225</v>
@@ -27736,7 +27728,7 @@
     </row>
     <row r="224">
       <c r="A224" t="s" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B224" t="s" s="2">
         <v>226</v>
@@ -27850,7 +27842,7 @@
     </row>
     <row r="225">
       <c r="A225" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B225" t="s" s="2">
         <v>227</v>
@@ -27966,7 +27958,7 @@
     </row>
     <row r="226">
       <c r="A226" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B226" t="s" s="2">
         <v>228</v>
@@ -28080,7 +28072,7 @@
     </row>
     <row r="227">
       <c r="A227" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B227" t="s" s="2">
         <v>233</v>
@@ -28194,7 +28186,7 @@
     </row>
     <row r="228">
       <c r="A228" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B228" t="s" s="2">
         <v>237</v>
@@ -28308,7 +28300,7 @@
     </row>
     <row r="229">
       <c r="A229" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B229" t="s" s="2">
         <v>240</v>
@@ -28422,7 +28414,7 @@
     </row>
     <row r="230">
       <c r="A230" t="s" s="2">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B230" t="s" s="2">
         <v>243</v>
@@ -28536,7 +28528,7 @@
     </row>
     <row r="231">
       <c r="A231" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B231" t="s" s="2">
         <v>246</v>
@@ -28650,7 +28642,7 @@
     </row>
     <row r="232">
       <c r="A232" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B232" t="s" s="2">
         <v>249</v>
@@ -28762,7 +28754,7 @@
     </row>
     <row r="233">
       <c r="A233" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B233" t="s" s="2">
         <v>253</v>
@@ -28874,7 +28866,7 @@
     </row>
     <row r="234">
       <c r="A234" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B234" t="s" s="2">
         <v>254</v>
@@ -28988,7 +28980,7 @@
     </row>
     <row r="235">
       <c r="A235" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B235" t="s" s="2">
         <v>255</v>
@@ -29104,7 +29096,7 @@
     </row>
     <row r="236">
       <c r="A236" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B236" t="s" s="2">
         <v>256</v>
@@ -29218,7 +29210,7 @@
     </row>
     <row r="237">
       <c r="A237" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B237" t="s" s="2">
         <v>259</v>
@@ -29332,7 +29324,7 @@
     </row>
     <row r="238">
       <c r="A238" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B238" t="s" s="2">
         <v>262</v>
@@ -29446,7 +29438,7 @@
     </row>
     <row r="239">
       <c r="A239" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B239" t="s" s="2">
         <v>266</v>
@@ -29560,7 +29552,7 @@
     </row>
     <row r="240">
       <c r="A240" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B240" t="s" s="2">
         <v>270</v>
@@ -29674,13 +29666,13 @@
     </row>
     <row r="241">
       <c r="A241" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B241" t="s" s="2">
         <v>183</v>
       </c>
       <c r="C241" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D241" t="s" s="2">
         <v>77</v>
@@ -29788,7 +29780,7 @@
     </row>
     <row r="242">
       <c r="A242" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B242" t="s" s="2">
         <v>188</v>
@@ -29900,7 +29892,7 @@
     </row>
     <row r="243">
       <c r="A243" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B243" t="s" s="2">
         <v>189</v>
@@ -30014,7 +30006,7 @@
     </row>
     <row r="244">
       <c r="A244" t="s" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B244" t="s" s="2">
         <v>190</v>
@@ -30130,7 +30122,7 @@
     </row>
     <row r="245">
       <c r="A245" t="s" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B245" t="s" s="2">
         <v>191</v>
@@ -30242,7 +30234,7 @@
     </row>
     <row r="246">
       <c r="A246" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B246" t="s" s="2">
         <v>194</v>
@@ -30356,7 +30348,7 @@
     </row>
     <row r="247">
       <c r="A247" t="s" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B247" t="s" s="2">
         <v>198</v>
@@ -30382,13 +30374,13 @@
         <v>77</v>
       </c>
       <c r="K247" t="s" s="2">
+        <v>504</v>
+      </c>
+      <c r="L247" t="s" s="2">
         <v>505</v>
       </c>
-      <c r="L247" t="s" s="2">
+      <c r="M247" t="s" s="2">
         <v>506</v>
-      </c>
-      <c r="M247" t="s" s="2">
-        <v>507</v>
       </c>
       <c r="N247" s="2"/>
       <c r="O247" s="2"/>
@@ -30451,13 +30443,13 @@
         <v>77</v>
       </c>
       <c r="AJ247" t="s" s="2">
-        <v>285</v>
+        <v>77</v>
       </c>
       <c r="AK247" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AL247" t="s" s="2">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="AM247" t="s" s="2">
         <v>77</v>
@@ -30468,7 +30460,7 @@
     </row>
     <row r="248">
       <c r="A248" t="s" s="2">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B248" t="s" s="2">
         <v>203</v>
@@ -30580,7 +30572,7 @@
     </row>
     <row r="249">
       <c r="A249" t="s" s="2">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B249" t="s" s="2">
         <v>207</v>
@@ -30692,7 +30684,7 @@
     </row>
     <row r="250">
       <c r="A250" t="s" s="2">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B250" t="s" s="2">
         <v>208</v>
@@ -30806,7 +30798,7 @@
     </row>
     <row r="251">
       <c r="A251" t="s" s="2">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B251" t="s" s="2">
         <v>209</v>
@@ -30922,7 +30914,7 @@
     </row>
     <row r="252">
       <c r="A252" t="s" s="2">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B252" t="s" s="2">
         <v>210</v>
@@ -30968,7 +30960,7 @@
         <v>77</v>
       </c>
       <c r="S252" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T252" t="s" s="2">
         <v>77</v>
@@ -31036,7 +31028,7 @@
     </row>
     <row r="253">
       <c r="A253" t="s" s="2">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B253" t="s" s="2">
         <v>216</v>
@@ -31150,7 +31142,7 @@
     </row>
     <row r="254">
       <c r="A254" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B254" t="s" s="2">
         <v>221</v>
@@ -31262,7 +31254,7 @@
     </row>
     <row r="255">
       <c r="A255" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B255" t="s" s="2">
         <v>225</v>
@@ -31374,7 +31366,7 @@
     </row>
     <row r="256">
       <c r="A256" t="s" s="2">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B256" t="s" s="2">
         <v>226</v>
@@ -31488,7 +31480,7 @@
     </row>
     <row r="257">
       <c r="A257" t="s" s="2">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B257" t="s" s="2">
         <v>227</v>
@@ -31604,7 +31596,7 @@
     </row>
     <row r="258">
       <c r="A258" t="s" s="2">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B258" t="s" s="2">
         <v>228</v>
@@ -31718,7 +31710,7 @@
     </row>
     <row r="259">
       <c r="A259" t="s" s="2">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B259" t="s" s="2">
         <v>233</v>
@@ -31832,7 +31824,7 @@
     </row>
     <row r="260">
       <c r="A260" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B260" t="s" s="2">
         <v>237</v>
@@ -31946,7 +31938,7 @@
     </row>
     <row r="261">
       <c r="A261" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B261" t="s" s="2">
         <v>240</v>
@@ -32060,7 +32052,7 @@
     </row>
     <row r="262">
       <c r="A262" t="s" s="2">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B262" t="s" s="2">
         <v>243</v>
@@ -32174,7 +32166,7 @@
     </row>
     <row r="263">
       <c r="A263" t="s" s="2">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B263" t="s" s="2">
         <v>246</v>
@@ -32288,7 +32280,7 @@
     </row>
     <row r="264">
       <c r="A264" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B264" t="s" s="2">
         <v>249</v>
@@ -32400,7 +32392,7 @@
     </row>
     <row r="265">
       <c r="A265" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B265" t="s" s="2">
         <v>253</v>
@@ -32512,7 +32504,7 @@
     </row>
     <row r="266">
       <c r="A266" t="s" s="2">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B266" t="s" s="2">
         <v>254</v>
@@ -32626,7 +32618,7 @@
     </row>
     <row r="267">
       <c r="A267" t="s" s="2">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B267" t="s" s="2">
         <v>255</v>
@@ -32742,7 +32734,7 @@
     </row>
     <row r="268">
       <c r="A268" t="s" s="2">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B268" t="s" s="2">
         <v>256</v>
@@ -32856,7 +32848,7 @@
     </row>
     <row r="269">
       <c r="A269" t="s" s="2">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B269" t="s" s="2">
         <v>259</v>
@@ -32970,7 +32962,7 @@
     </row>
     <row r="270">
       <c r="A270" t="s" s="2">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B270" t="s" s="2">
         <v>262</v>
@@ -33084,7 +33076,7 @@
     </row>
     <row r="271">
       <c r="A271" t="s" s="2">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B271" t="s" s="2">
         <v>266</v>
@@ -33198,7 +33190,7 @@
     </row>
     <row r="272">
       <c r="A272" t="s" s="2">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B272" t="s" s="2">
         <v>270</v>
@@ -33312,13 +33304,13 @@
     </row>
     <row r="273">
       <c r="A273" t="s" s="2">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B273" t="s" s="2">
         <v>183</v>
       </c>
       <c r="C273" t="s" s="2">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D273" t="s" s="2">
         <v>77</v>
@@ -33426,7 +33418,7 @@
     </row>
     <row r="274">
       <c r="A274" t="s" s="2">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B274" t="s" s="2">
         <v>188</v>
@@ -33538,7 +33530,7 @@
     </row>
     <row r="275">
       <c r="A275" t="s" s="2">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B275" t="s" s="2">
         <v>189</v>
@@ -33652,7 +33644,7 @@
     </row>
     <row r="276">
       <c r="A276" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B276" t="s" s="2">
         <v>190</v>
@@ -33768,7 +33760,7 @@
     </row>
     <row r="277">
       <c r="A277" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B277" t="s" s="2">
         <v>191</v>
@@ -33880,7 +33872,7 @@
     </row>
     <row r="278">
       <c r="A278" t="s" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B278" t="s" s="2">
         <v>194</v>
@@ -33994,7 +33986,7 @@
     </row>
     <row r="279">
       <c r="A279" t="s" s="2">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B279" t="s" s="2">
         <v>198</v>
@@ -34020,13 +34012,13 @@
         <v>77</v>
       </c>
       <c r="K279" t="s" s="2">
+        <v>541</v>
+      </c>
+      <c r="L279" t="s" s="2">
         <v>542</v>
       </c>
-      <c r="L279" t="s" s="2">
+      <c r="M279" t="s" s="2">
         <v>543</v>
-      </c>
-      <c r="M279" t="s" s="2">
-        <v>544</v>
       </c>
       <c r="N279" s="2"/>
       <c r="O279" s="2"/>
@@ -34089,13 +34081,13 @@
         <v>77</v>
       </c>
       <c r="AJ279" t="s" s="2">
-        <v>285</v>
+        <v>77</v>
       </c>
       <c r="AK279" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AL279" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AM279" t="s" s="2">
         <v>77</v>
@@ -34106,7 +34098,7 @@
     </row>
     <row r="280">
       <c r="A280" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B280" t="s" s="2">
         <v>203</v>
@@ -34218,7 +34210,7 @@
     </row>
     <row r="281">
       <c r="A281" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B281" t="s" s="2">
         <v>207</v>
@@ -34330,7 +34322,7 @@
     </row>
     <row r="282">
       <c r="A282" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B282" t="s" s="2">
         <v>208</v>
@@ -34444,7 +34436,7 @@
     </row>
     <row r="283">
       <c r="A283" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B283" t="s" s="2">
         <v>209</v>
@@ -34560,7 +34552,7 @@
     </row>
     <row r="284">
       <c r="A284" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B284" t="s" s="2">
         <v>210</v>
@@ -34606,7 +34598,7 @@
         <v>77</v>
       </c>
       <c r="S284" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T284" t="s" s="2">
         <v>77</v>
@@ -34674,7 +34666,7 @@
     </row>
     <row r="285">
       <c r="A285" t="s" s="2">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B285" t="s" s="2">
         <v>216</v>
@@ -34788,7 +34780,7 @@
     </row>
     <row r="286">
       <c r="A286" t="s" s="2">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B286" t="s" s="2">
         <v>221</v>
@@ -34900,7 +34892,7 @@
     </row>
     <row r="287">
       <c r="A287" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B287" t="s" s="2">
         <v>225</v>
@@ -35012,7 +35004,7 @@
     </row>
     <row r="288">
       <c r="A288" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B288" t="s" s="2">
         <v>226</v>
@@ -35126,7 +35118,7 @@
     </row>
     <row r="289">
       <c r="A289" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B289" t="s" s="2">
         <v>227</v>
@@ -35242,7 +35234,7 @@
     </row>
     <row r="290">
       <c r="A290" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B290" t="s" s="2">
         <v>228</v>
@@ -35356,7 +35348,7 @@
     </row>
     <row r="291">
       <c r="A291" t="s" s="2">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B291" t="s" s="2">
         <v>233</v>
@@ -35470,7 +35462,7 @@
     </row>
     <row r="292">
       <c r="A292" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B292" t="s" s="2">
         <v>237</v>
@@ -35584,7 +35576,7 @@
     </row>
     <row r="293">
       <c r="A293" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B293" t="s" s="2">
         <v>240</v>
@@ -35698,7 +35690,7 @@
     </row>
     <row r="294">
       <c r="A294" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B294" t="s" s="2">
         <v>243</v>
@@ -35812,7 +35804,7 @@
     </row>
     <row r="295">
       <c r="A295" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B295" t="s" s="2">
         <v>246</v>
@@ -35926,7 +35918,7 @@
     </row>
     <row r="296">
       <c r="A296" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B296" t="s" s="2">
         <v>249</v>
@@ -36038,7 +36030,7 @@
     </row>
     <row r="297">
       <c r="A297" t="s" s="2">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B297" t="s" s="2">
         <v>253</v>
@@ -36150,7 +36142,7 @@
     </row>
     <row r="298">
       <c r="A298" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B298" t="s" s="2">
         <v>254</v>
@@ -36264,7 +36256,7 @@
     </row>
     <row r="299">
       <c r="A299" t="s" s="2">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B299" t="s" s="2">
         <v>255</v>
@@ -36380,7 +36372,7 @@
     </row>
     <row r="300">
       <c r="A300" t="s" s="2">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B300" t="s" s="2">
         <v>256</v>
@@ -36494,7 +36486,7 @@
     </row>
     <row r="301">
       <c r="A301" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B301" t="s" s="2">
         <v>259</v>
@@ -36608,7 +36600,7 @@
     </row>
     <row r="302">
       <c r="A302" t="s" s="2">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B302" t="s" s="2">
         <v>262</v>
@@ -36722,7 +36714,7 @@
     </row>
     <row r="303">
       <c r="A303" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B303" t="s" s="2">
         <v>266</v>
@@ -36836,7 +36828,7 @@
     </row>
     <row r="304">
       <c r="A304" t="s" s="2">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B304" t="s" s="2">
         <v>270</v>
@@ -36950,13 +36942,13 @@
     </row>
     <row r="305">
       <c r="A305" t="s" s="2">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B305" t="s" s="2">
         <v>183</v>
       </c>
       <c r="C305" t="s" s="2">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D305" t="s" s="2">
         <v>77</v>
@@ -37064,7 +37056,7 @@
     </row>
     <row r="306">
       <c r="A306" t="s" s="2">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B306" t="s" s="2">
         <v>188</v>
@@ -37176,7 +37168,7 @@
     </row>
     <row r="307">
       <c r="A307" t="s" s="2">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B307" t="s" s="2">
         <v>189</v>
@@ -37290,7 +37282,7 @@
     </row>
     <row r="308">
       <c r="A308" t="s" s="2">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B308" t="s" s="2">
         <v>190</v>
@@ -37406,7 +37398,7 @@
     </row>
     <row r="309">
       <c r="A309" t="s" s="2">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B309" t="s" s="2">
         <v>191</v>
@@ -37518,7 +37510,7 @@
     </row>
     <row r="310">
       <c r="A310" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B310" t="s" s="2">
         <v>194</v>
@@ -37632,7 +37624,7 @@
     </row>
     <row r="311">
       <c r="A311" t="s" s="2">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B311" t="s" s="2">
         <v>198</v>
@@ -37658,13 +37650,13 @@
         <v>77</v>
       </c>
       <c r="K311" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="L311" t="s" s="2">
         <v>579</v>
       </c>
-      <c r="L311" t="s" s="2">
+      <c r="M311" t="s" s="2">
         <v>580</v>
-      </c>
-      <c r="M311" t="s" s="2">
-        <v>581</v>
       </c>
       <c r="N311" s="2"/>
       <c r="O311" s="2"/>
@@ -37727,13 +37719,13 @@
         <v>77</v>
       </c>
       <c r="AJ311" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AK311" t="s" s="2">
+        <v>581</v>
+      </c>
+      <c r="AL311" t="s" s="2">
         <v>582</v>
-      </c>
-      <c r="AK311" t="s" s="2">
-        <v>583</v>
-      </c>
-      <c r="AL311" t="s" s="2">
-        <v>584</v>
       </c>
       <c r="AM311" t="s" s="2">
         <v>77</v>
@@ -37744,7 +37736,7 @@
     </row>
     <row r="312">
       <c r="A312" t="s" s="2">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B312" t="s" s="2">
         <v>203</v>
@@ -37856,7 +37848,7 @@
     </row>
     <row r="313">
       <c r="A313" t="s" s="2">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B313" t="s" s="2">
         <v>207</v>
@@ -37968,7 +37960,7 @@
     </row>
     <row r="314">
       <c r="A314" t="s" s="2">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B314" t="s" s="2">
         <v>208</v>
@@ -38082,7 +38074,7 @@
     </row>
     <row r="315">
       <c r="A315" t="s" s="2">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B315" t="s" s="2">
         <v>209</v>
@@ -38198,7 +38190,7 @@
     </row>
     <row r="316">
       <c r="A316" t="s" s="2">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B316" t="s" s="2">
         <v>210</v>
@@ -38244,7 +38236,7 @@
         <v>77</v>
       </c>
       <c r="S316" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T316" t="s" s="2">
         <v>77</v>
@@ -38312,7 +38304,7 @@
     </row>
     <row r="317">
       <c r="A317" t="s" s="2">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B317" t="s" s="2">
         <v>216</v>
@@ -38426,7 +38418,7 @@
     </row>
     <row r="318">
       <c r="A318" t="s" s="2">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B318" t="s" s="2">
         <v>221</v>
@@ -38538,7 +38530,7 @@
     </row>
     <row r="319">
       <c r="A319" t="s" s="2">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B319" t="s" s="2">
         <v>225</v>
@@ -38650,7 +38642,7 @@
     </row>
     <row r="320">
       <c r="A320" t="s" s="2">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B320" t="s" s="2">
         <v>226</v>
@@ -38764,7 +38756,7 @@
     </row>
     <row r="321">
       <c r="A321" t="s" s="2">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B321" t="s" s="2">
         <v>227</v>
@@ -38880,7 +38872,7 @@
     </row>
     <row r="322">
       <c r="A322" t="s" s="2">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B322" t="s" s="2">
         <v>228</v>
@@ -38994,7 +38986,7 @@
     </row>
     <row r="323">
       <c r="A323" t="s" s="2">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B323" t="s" s="2">
         <v>233</v>
@@ -39108,7 +39100,7 @@
     </row>
     <row r="324">
       <c r="A324" t="s" s="2">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B324" t="s" s="2">
         <v>237</v>
@@ -39222,7 +39214,7 @@
     </row>
     <row r="325">
       <c r="A325" t="s" s="2">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B325" t="s" s="2">
         <v>240</v>
@@ -39336,7 +39328,7 @@
     </row>
     <row r="326">
       <c r="A326" t="s" s="2">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B326" t="s" s="2">
         <v>243</v>
@@ -39450,7 +39442,7 @@
     </row>
     <row r="327">
       <c r="A327" t="s" s="2">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B327" t="s" s="2">
         <v>246</v>
@@ -39564,7 +39556,7 @@
     </row>
     <row r="328">
       <c r="A328" t="s" s="2">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B328" t="s" s="2">
         <v>249</v>
@@ -39676,7 +39668,7 @@
     </row>
     <row r="329">
       <c r="A329" t="s" s="2">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B329" t="s" s="2">
         <v>253</v>
@@ -39788,7 +39780,7 @@
     </row>
     <row r="330">
       <c r="A330" t="s" s="2">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B330" t="s" s="2">
         <v>254</v>
@@ -39902,7 +39894,7 @@
     </row>
     <row r="331">
       <c r="A331" t="s" s="2">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B331" t="s" s="2">
         <v>255</v>
@@ -40018,7 +40010,7 @@
     </row>
     <row r="332">
       <c r="A332" t="s" s="2">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B332" t="s" s="2">
         <v>256</v>
@@ -40132,7 +40124,7 @@
     </row>
     <row r="333">
       <c r="A333" t="s" s="2">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B333" t="s" s="2">
         <v>259</v>
@@ -40246,7 +40238,7 @@
     </row>
     <row r="334">
       <c r="A334" t="s" s="2">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B334" t="s" s="2">
         <v>262</v>
@@ -40360,7 +40352,7 @@
     </row>
     <row r="335">
       <c r="A335" t="s" s="2">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B335" t="s" s="2">
         <v>266</v>
@@ -40474,7 +40466,7 @@
     </row>
     <row r="336">
       <c r="A336" t="s" s="2">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B336" t="s" s="2">
         <v>270</v>
@@ -40588,13 +40580,13 @@
     </row>
     <row r="337">
       <c r="A337" t="s" s="2">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B337" t="s" s="2">
         <v>183</v>
       </c>
       <c r="C337" t="s" s="2">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D337" t="s" s="2">
         <v>77</v>
@@ -40702,7 +40694,7 @@
     </row>
     <row r="338">
       <c r="A338" t="s" s="2">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B338" t="s" s="2">
         <v>188</v>
@@ -40814,7 +40806,7 @@
     </row>
     <row r="339">
       <c r="A339" t="s" s="2">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B339" t="s" s="2">
         <v>189</v>
@@ -40928,7 +40920,7 @@
     </row>
     <row r="340">
       <c r="A340" t="s" s="2">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B340" t="s" s="2">
         <v>190</v>
@@ -41044,7 +41036,7 @@
     </row>
     <row r="341">
       <c r="A341" t="s" s="2">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B341" t="s" s="2">
         <v>191</v>
@@ -41156,7 +41148,7 @@
     </row>
     <row r="342">
       <c r="A342" t="s" s="2">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B342" t="s" s="2">
         <v>194</v>
@@ -41270,7 +41262,7 @@
     </row>
     <row r="343">
       <c r="A343" t="s" s="2">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B343" t="s" s="2">
         <v>198</v>
@@ -41296,13 +41288,13 @@
         <v>77</v>
       </c>
       <c r="K343" t="s" s="2">
+        <v>616</v>
+      </c>
+      <c r="L343" t="s" s="2">
+        <v>617</v>
+      </c>
+      <c r="M343" t="s" s="2">
         <v>618</v>
-      </c>
-      <c r="L343" t="s" s="2">
-        <v>619</v>
-      </c>
-      <c r="M343" t="s" s="2">
-        <v>620</v>
       </c>
       <c r="N343" s="2"/>
       <c r="O343" s="2"/>
@@ -41365,13 +41357,13 @@
         <v>77</v>
       </c>
       <c r="AJ343" t="s" s="2">
-        <v>285</v>
+        <v>77</v>
       </c>
       <c r="AK343" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AL343" t="s" s="2">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="AM343" t="s" s="2">
         <v>77</v>
@@ -41382,7 +41374,7 @@
     </row>
     <row r="344">
       <c r="A344" t="s" s="2">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B344" t="s" s="2">
         <v>203</v>
@@ -41494,7 +41486,7 @@
     </row>
     <row r="345">
       <c r="A345" t="s" s="2">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B345" t="s" s="2">
         <v>207</v>
@@ -41606,7 +41598,7 @@
     </row>
     <row r="346">
       <c r="A346" t="s" s="2">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B346" t="s" s="2">
         <v>208</v>
@@ -41720,7 +41712,7 @@
     </row>
     <row r="347">
       <c r="A347" t="s" s="2">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B347" t="s" s="2">
         <v>209</v>
@@ -41836,7 +41828,7 @@
     </row>
     <row r="348">
       <c r="A348" t="s" s="2">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B348" t="s" s="2">
         <v>210</v>
@@ -41882,7 +41874,7 @@
         <v>77</v>
       </c>
       <c r="S348" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="T348" t="s" s="2">
         <v>77</v>
@@ -41950,7 +41942,7 @@
     </row>
     <row r="349">
       <c r="A349" t="s" s="2">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B349" t="s" s="2">
         <v>216</v>
@@ -42064,7 +42056,7 @@
     </row>
     <row r="350">
       <c r="A350" t="s" s="2">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B350" t="s" s="2">
         <v>221</v>
@@ -42176,7 +42168,7 @@
     </row>
     <row r="351">
       <c r="A351" t="s" s="2">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B351" t="s" s="2">
         <v>225</v>
@@ -42288,7 +42280,7 @@
     </row>
     <row r="352">
       <c r="A352" t="s" s="2">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B352" t="s" s="2">
         <v>226</v>
@@ -42402,7 +42394,7 @@
     </row>
     <row r="353">
       <c r="A353" t="s" s="2">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B353" t="s" s="2">
         <v>227</v>
@@ -42518,7 +42510,7 @@
     </row>
     <row r="354">
       <c r="A354" t="s" s="2">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B354" t="s" s="2">
         <v>228</v>
@@ -42632,7 +42624,7 @@
     </row>
     <row r="355">
       <c r="A355" t="s" s="2">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B355" t="s" s="2">
         <v>233</v>
@@ -42746,7 +42738,7 @@
     </row>
     <row r="356">
       <c r="A356" t="s" s="2">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B356" t="s" s="2">
         <v>237</v>
@@ -42860,7 +42852,7 @@
     </row>
     <row r="357">
       <c r="A357" t="s" s="2">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B357" t="s" s="2">
         <v>240</v>
@@ -42974,7 +42966,7 @@
     </row>
     <row r="358">
       <c r="A358" t="s" s="2">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B358" t="s" s="2">
         <v>243</v>
@@ -43088,7 +43080,7 @@
     </row>
     <row r="359">
       <c r="A359" t="s" s="2">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B359" t="s" s="2">
         <v>246</v>
@@ -43202,7 +43194,7 @@
     </row>
     <row r="360">
       <c r="A360" t="s" s="2">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B360" t="s" s="2">
         <v>249</v>
@@ -43314,7 +43306,7 @@
     </row>
     <row r="361">
       <c r="A361" t="s" s="2">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B361" t="s" s="2">
         <v>253</v>
@@ -43426,7 +43418,7 @@
     </row>
     <row r="362">
       <c r="A362" t="s" s="2">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B362" t="s" s="2">
         <v>254</v>
@@ -43540,7 +43532,7 @@
     </row>
     <row r="363">
       <c r="A363" t="s" s="2">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B363" t="s" s="2">
         <v>255</v>
@@ -43656,7 +43648,7 @@
     </row>
     <row r="364">
       <c r="A364" t="s" s="2">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B364" t="s" s="2">
         <v>256</v>
@@ -43770,7 +43762,7 @@
     </row>
     <row r="365">
       <c r="A365" t="s" s="2">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B365" t="s" s="2">
         <v>259</v>
@@ -43884,7 +43876,7 @@
     </row>
     <row r="366">
       <c r="A366" t="s" s="2">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B366" t="s" s="2">
         <v>262</v>
@@ -43998,7 +43990,7 @@
     </row>
     <row r="367">
       <c r="A367" t="s" s="2">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B367" t="s" s="2">
         <v>266</v>
@@ -44112,7 +44104,7 @@
     </row>
     <row r="368">
       <c r="A368" t="s" s="2">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B368" t="s" s="2">
         <v>270</v>
@@ -44226,10 +44218,10 @@
     </row>
     <row r="369">
       <c r="A369" t="s" s="2">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B369" t="s" s="2">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C369" s="2"/>
       <c r="D369" t="s" s="2">
@@ -44252,19 +44244,19 @@
         <v>88</v>
       </c>
       <c r="K369" t="s" s="2">
+        <v>646</v>
+      </c>
+      <c r="L369" t="s" s="2">
+        <v>647</v>
+      </c>
+      <c r="M369" t="s" s="2">
         <v>648</v>
       </c>
-      <c r="L369" t="s" s="2">
+      <c r="N369" t="s" s="2">
         <v>649</v>
       </c>
-      <c r="M369" t="s" s="2">
+      <c r="O369" t="s" s="2">
         <v>650</v>
-      </c>
-      <c r="N369" t="s" s="2">
-        <v>651</v>
-      </c>
-      <c r="O369" t="s" s="2">
-        <v>652</v>
       </c>
       <c r="P369" t="s" s="2">
         <v>77</v>
@@ -44313,7 +44305,7 @@
         <v>77</v>
       </c>
       <c r="AF369" t="s" s="2">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="AG369" t="s" s="2">
         <v>78</v>

</xml_diff>